<commit_message>
Added the reporting piece
</commit_message>
<xml_diff>
--- a/src/main/java/framework/auto/xls/Google.xlsx
+++ b/src/main/java/framework/auto/xls/Google.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11115" windowHeight="3135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12465" windowHeight="2730" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manual_TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="3" r:id="rId2"/>
     <sheet name="GoogleSearch" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Test case number (optional)</t>
   </si>
@@ -193,9 +194,6 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>1. Enter valid inputs (First Name, 
      Last Name, 
      Email,
@@ -273,12 +271,19 @@
   <si>
     <t>STeP-IN</t>
   </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -882,16 +887,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="33.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="13" width="19" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="22.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="30.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="21.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="23.5703125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="3" width="33.140625" collapsed="true"/>
+    <col min="9" max="9" style="3" width="9.140625" collapsed="true"/>
+    <col min="10" max="13" customWidth="true" style="3" width="19.0" collapsed="true"/>
+    <col min="14" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -955,10 +960,10 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
@@ -988,10 +993,10 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
@@ -1149,15 +1154,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1174,21 +1180,23 @@
         <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1201,44 +1209,47 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E2" s="9"/>
     </row>
   </sheetData>

</xml_diff>